<commit_message>
updated type_calc/orig to type_reclass/main
</commit_message>
<xml_diff>
--- a/data/input/infos_from_ndcs_default.xlsx
+++ b/data/input/infos_from_ndcs_default.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annikag\primap\ndc_quantifications\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annikag\primap\save_newcode_newpreprocess\ndc_quantifications\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8030" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13425" windowHeight="5655"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -8026,12 +8026,6 @@
     <t>submission_date</t>
   </si>
   <si>
-    <t>type_calc.mod</t>
-  </si>
-  <si>
-    <t>type_orig.mod</t>
-  </si>
-  <si>
     <t>type_long (possible types: NGT, RBY, ABS, RBU, ABU, REI, AEI)</t>
   </si>
   <si>
@@ -9738,6 +9732,12 @@
   </si>
   <si>
     <t>[p. 11-12] "Combined, the energy (excluding transport) and Land Use Land Use Change and Forestry sectors account for approximately 36% of national emissions in 2000, and 26% of emissions in 2030 under Business As Usual. Under the business as usual case, the Land Use Land Use Change and 12 Forestry sector continues to be a net emitter. [...] The additional mitigation ambition (section 3.2) also covers agriculture and transport. Combined, the transport and agriculture sectors represent a further 62% of national emissions in 2000, and 70% of emissions in 2030 under Business As Usual."</t>
+  </si>
+  <si>
+    <t>type_reclass.mod</t>
+  </si>
+  <si>
+    <t>type_main.mod</t>
   </si>
 </sst>
 </file>
@@ -10372,24 +10372,24 @@
   <dimension ref="A1:GO43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3080" ySplit="2280" topLeftCell="DD22" activePane="bottomRight"/>
+      <pane xSplit="3075" ySplit="2280" topLeftCell="DD6" activePane="bottomLeft"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="FC1" sqref="FC1"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD28"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" activeCell="DD31" sqref="DD31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" style="16" customWidth="1"/>
-    <col min="3" max="73" width="13.81640625" style="5" customWidth="1"/>
-    <col min="74" max="74" width="13.81640625" style="16" customWidth="1"/>
-    <col min="75" max="197" width="13.81640625" style="5" customWidth="1"/>
-    <col min="198" max="16384" width="9.1796875" style="5"/>
+    <col min="1" max="1" width="30.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="16" customWidth="1"/>
+    <col min="3" max="73" width="13.85546875" style="5" customWidth="1"/>
+    <col min="74" max="74" width="13.85546875" style="16" customWidth="1"/>
+    <col min="75" max="197" width="13.85546875" style="5" customWidth="1"/>
+    <col min="198" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>754</v>
       </c>
@@ -10520,7 +10520,7 @@
         <v>440</v>
       </c>
       <c r="AR1" s="41" t="s">
-        <v>2376</v>
+        <v>2374</v>
       </c>
       <c r="AS1" s="41" t="s">
         <v>441</v>
@@ -10982,7 +10982,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="2" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>741</v>
       </c>
@@ -11575,7 +11575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2215</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2216</v>
       </c>
@@ -12761,7 +12761,7 @@
         <v>42648</v>
       </c>
     </row>
-    <row r="5" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>755</v>
       </c>
@@ -13354,9 +13354,9 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2217</v>
+        <v>2568</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>396</v>
@@ -13947,9 +13947,9 @@
         <v>394</v>
       </c>
     </row>
-    <row r="7" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2218</v>
+        <v>2569</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>705</v>
@@ -14540,9 +14540,9 @@
         <v>394</v>
       </c>
     </row>
-    <row r="8" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>397</v>
@@ -14596,7 +14596,7 @@
         <v>1847</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>2449</v>
+        <v>2447</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>1673</v>
@@ -14644,7 +14644,7 @@
         <v>1982</v>
       </c>
       <c r="AI8" s="9" t="s">
-        <v>2445</v>
+        <v>2443</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>1740</v>
@@ -14656,7 +14656,7 @@
         <v>1686</v>
       </c>
       <c r="AM8" s="2" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
       <c r="AN8" s="2" t="s">
         <v>2190</v>
@@ -14674,7 +14674,7 @@
         <v>1448</v>
       </c>
       <c r="AS8" s="14" t="s">
-        <v>2316</v>
+        <v>2314</v>
       </c>
       <c r="AT8" s="2" t="s">
         <v>1573</v>
@@ -14886,7 +14886,7 @@
         <v>1891</v>
       </c>
       <c r="DM8" s="2" t="s">
-        <v>2310</v>
+        <v>2308</v>
       </c>
       <c r="DN8" s="9" t="s">
         <v>1553</v>
@@ -14907,7 +14907,7 @@
         <v>1906</v>
       </c>
       <c r="DT8" s="9" t="s">
-        <v>2311</v>
+        <v>2309</v>
       </c>
       <c r="DU8" s="2" t="s">
         <v>1344</v>
@@ -14958,7 +14958,7 @@
         <v>1044</v>
       </c>
       <c r="EK8" s="2" t="s">
-        <v>2317</v>
+        <v>2315</v>
       </c>
       <c r="EL8" s="2" t="s">
         <v>2197</v>
@@ -14982,7 +14982,7 @@
         <v>1720</v>
       </c>
       <c r="ES8" s="2" t="s">
-        <v>2370</v>
+        <v>2368</v>
       </c>
       <c r="ET8" s="9" t="s">
         <v>1198</v>
@@ -15012,7 +15012,7 @@
         <v>1111</v>
       </c>
       <c r="FC8" s="2" t="s">
-        <v>2568</v>
+        <v>2566</v>
       </c>
       <c r="FD8" s="2" t="s">
         <v>2188</v>
@@ -15073,9 +15073,9 @@
       <c r="GN8" s="9"/>
       <c r="GO8" s="9"/>
     </row>
-    <row r="9" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>2220</v>
+        <v>2218</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>594</v>
@@ -15652,9 +15652,9 @@
         <v>596</v>
       </c>
     </row>
-    <row r="10" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>2221</v>
+        <v>2219</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>603</v>
@@ -16231,9 +16231,9 @@
         <v>605</v>
       </c>
     </row>
-    <row r="11" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>612</v>
@@ -16824,9 +16824,9 @@
         <v>612</v>
       </c>
     </row>
-    <row r="12" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>195</v>
@@ -17417,9 +17417,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>2223</v>
+        <v>2221</v>
       </c>
       <c r="B13" s="2">
         <v>8</v>
@@ -17954,9 +17954,9 @@
       <c r="GN13" s="2"/>
       <c r="GO13" s="2"/>
     </row>
-    <row r="14" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -18160,513 +18160,513 @@
       <c r="GN14" s="2"/>
       <c r="GO14" s="2"/>
     </row>
-    <row r="15" spans="1:197" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:197" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>2253</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>2255</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>2257</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>2259</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>2261</v>
-      </c>
       <c r="F15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>2262</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>2264</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>2266</v>
-      </c>
       <c r="I15" s="14" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="K15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="L15" s="33" t="s">
+        <v>2264</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="N15" s="14" t="s">
         <v>2262</v>
       </c>
-      <c r="L15" s="33" t="s">
-        <v>2266</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="N15" s="14" t="s">
+      <c r="O15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="T15" s="46" t="s">
+        <v>2265</v>
+      </c>
+      <c r="U15" s="14" t="s">
         <v>2264</v>
       </c>
-      <c r="O15" s="14" t="s">
+      <c r="V15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="W15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="X15" s="14" t="s">
+        <v>2269</v>
+      </c>
+      <c r="Y15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="Z15" s="14" t="s">
+        <v>2272</v>
+      </c>
+      <c r="AA15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AB15" s="14" t="s">
+        <v>2274</v>
+      </c>
+      <c r="AC15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AD15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AE15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AF15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AG15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="AH15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AI15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AJ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AK15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AL15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="AM15" s="14" t="s">
+        <v>2276</v>
+      </c>
+      <c r="AN15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="AO15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="AP15" s="14" t="s">
+        <v>2277</v>
+      </c>
+      <c r="AQ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AR15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AS15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AT15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AU15" s="14" t="s">
+        <v>2255</v>
+      </c>
+      <c r="AV15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AW15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AX15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="AY15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="AZ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BA15" s="14" t="s">
+        <v>2272</v>
+      </c>
+      <c r="BB15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="BC15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BD15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="BE15" s="14" t="s">
+        <v>2274</v>
+      </c>
+      <c r="BF15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BG15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BH15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="BI15" s="14" t="s">
+        <v>2283</v>
+      </c>
+      <c r="BJ15" s="14" t="s">
+        <v>2253</v>
+      </c>
+      <c r="BK15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="BL15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BM15" s="14" t="s">
+        <v>2253</v>
+      </c>
+      <c r="BN15" s="14" t="s">
+        <v>2255</v>
+      </c>
+      <c r="BO15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BP15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BQ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BR15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="BS15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BT15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BU15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BV15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="BW15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="BX15" s="14" t="s">
+        <v>2285</v>
+      </c>
+      <c r="BY15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="BZ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CA15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CB15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="CC15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="CD15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CE15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="CF15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CG15" s="14" t="s">
+        <v>2285</v>
+      </c>
+      <c r="CH15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CI15" s="14" t="s">
+        <v>2255</v>
+      </c>
+      <c r="CJ15" s="14" t="s">
+        <v>2277</v>
+      </c>
+      <c r="CK15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CL15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CM15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CN15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CO15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="CP15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="CQ15" s="14" t="s">
+        <v>2288</v>
+      </c>
+      <c r="CR15" s="14" t="s">
+        <v>2289</v>
+      </c>
+      <c r="CS15" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="CT15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="CU15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="CV15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CW15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CX15" s="14" t="s">
+        <v>2277</v>
+      </c>
+      <c r="CY15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CZ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DA15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DB15" s="14" t="s">
+        <v>2272</v>
+      </c>
+      <c r="DC15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DD15" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="DE15" s="14" t="s">
+        <v>2291</v>
+      </c>
+      <c r="DF15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="DG15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DH15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DI15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="DJ15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="DK15" s="33" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DL15" s="14" t="s">
+        <v>2259</v>
+      </c>
+      <c r="DM15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="DN15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DO15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="DP15" s="14" t="s">
+        <v>2255</v>
+      </c>
+      <c r="DQ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DR15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DS15" s="14" t="s">
+        <v>2277</v>
+      </c>
+      <c r="DT15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DU15" s="14" t="s">
+        <v>2277</v>
+      </c>
+      <c r="DV15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DW15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="DX15" s="14" t="s">
+        <v>2255</v>
+      </c>
+      <c r="DY15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="DZ15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="EA15" s="14" t="s">
+        <v>2293</v>
+      </c>
+      <c r="EB15" s="14" t="s">
+        <v>2272</v>
+      </c>
+      <c r="EC15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="ED15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="EE15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="EF15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="EG15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="EH15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="EI15" s="14" t="s">
+        <v>2267</v>
+      </c>
+      <c r="EJ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="EK15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="EL15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="EM15" s="14" t="s">
+        <v>2294</v>
+      </c>
+      <c r="EN15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="EO15" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="EP15" s="14" t="s">
+        <v>2271</v>
+      </c>
+      <c r="EQ15" s="14" t="s">
+        <v>2291</v>
+      </c>
+      <c r="ER15" s="14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="ES15" s="14" t="s">
+        <v>2253</v>
+      </c>
+      <c r="ET15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="EU15" s="14" t="s">
+        <v>2269</v>
+      </c>
+      <c r="EV15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="EW15" s="14" t="s">
         <v>2262</v>
       </c>
-      <c r="P15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="Q15" s="14" t="s">
-        <v>2267</v>
-      </c>
-      <c r="R15" s="14" t="s">
-        <v>2267</v>
-      </c>
-      <c r="S15" s="14" t="s">
+      <c r="EX15" s="14" t="s">
         <v>2269</v>
       </c>
-      <c r="T15" s="46" t="s">
-        <v>2267</v>
-      </c>
-      <c r="U15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="V15" s="14" t="s">
+      <c r="EY15" s="14" t="s">
+        <v>2272</v>
+      </c>
+      <c r="EZ15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="FA15" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="FB15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="FC15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="FD15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="FE15" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="FF15" s="14" t="s">
+        <v>2255</v>
+      </c>
+      <c r="FG15" s="14" t="s">
+        <v>2296</v>
+      </c>
+      <c r="FH15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="FI15" s="14" t="s">
+        <v>2275</v>
+      </c>
+      <c r="FJ15" s="14" t="s">
         <v>2269</v>
       </c>
-      <c r="W15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="X15" s="14" t="s">
-        <v>2271</v>
-      </c>
-      <c r="Y15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="Z15" s="14" t="s">
-        <v>2274</v>
-      </c>
-      <c r="AA15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AB15" s="14" t="s">
-        <v>2276</v>
-      </c>
-      <c r="AC15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AD15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AE15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AF15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AG15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="AH15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AI15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AJ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AK15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AL15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="AM15" s="14" t="s">
-        <v>2278</v>
-      </c>
-      <c r="AN15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="AO15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="AP15" s="14" t="s">
-        <v>2279</v>
-      </c>
-      <c r="AQ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AR15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AS15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AT15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AU15" s="14" t="s">
-        <v>2257</v>
-      </c>
-      <c r="AV15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AW15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="AX15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="AY15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="AZ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BA15" s="14" t="s">
-        <v>2274</v>
-      </c>
-      <c r="BB15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="BC15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BD15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="BE15" s="14" t="s">
-        <v>2276</v>
-      </c>
-      <c r="BF15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BG15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BH15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="BI15" s="14" t="s">
-        <v>2285</v>
-      </c>
-      <c r="BJ15" s="14" t="s">
-        <v>2255</v>
-      </c>
-      <c r="BK15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="BL15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BM15" s="14" t="s">
-        <v>2255</v>
-      </c>
-      <c r="BN15" s="14" t="s">
-        <v>2257</v>
-      </c>
-      <c r="BO15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BP15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BQ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BR15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="BS15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BT15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BU15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BV15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="BW15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="BX15" s="14" t="s">
-        <v>2287</v>
-      </c>
-      <c r="BY15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="BZ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CA15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CB15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="CC15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="CD15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CE15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="CF15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CG15" s="14" t="s">
-        <v>2287</v>
-      </c>
-      <c r="CH15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CI15" s="14" t="s">
-        <v>2257</v>
-      </c>
-      <c r="CJ15" s="14" t="s">
-        <v>2279</v>
-      </c>
-      <c r="CK15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CL15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CM15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CN15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CO15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="CP15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="CQ15" s="14" t="s">
-        <v>2290</v>
-      </c>
-      <c r="CR15" s="14" t="s">
-        <v>2291</v>
-      </c>
-      <c r="CS15" s="14" t="s">
-        <v>2267</v>
-      </c>
-      <c r="CT15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="CU15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="CV15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CW15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CX15" s="14" t="s">
-        <v>2279</v>
-      </c>
-      <c r="CY15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="CZ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DA15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DB15" s="14" t="s">
-        <v>2274</v>
-      </c>
-      <c r="DC15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DD15" s="14" t="s">
-        <v>2267</v>
-      </c>
-      <c r="DE15" s="14" t="s">
-        <v>2293</v>
-      </c>
-      <c r="DF15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="DG15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DH15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DI15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="DJ15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="DK15" s="33" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DL15" s="14" t="s">
-        <v>2261</v>
-      </c>
-      <c r="DM15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="DN15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DO15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="DP15" s="14" t="s">
-        <v>2257</v>
-      </c>
-      <c r="DQ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DR15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DS15" s="14" t="s">
-        <v>2279</v>
-      </c>
-      <c r="DT15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DU15" s="14" t="s">
-        <v>2279</v>
-      </c>
-      <c r="DV15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DW15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="DX15" s="14" t="s">
-        <v>2257</v>
-      </c>
-      <c r="DY15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="DZ15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="EA15" s="14" t="s">
-        <v>2295</v>
-      </c>
-      <c r="EB15" s="14" t="s">
-        <v>2274</v>
-      </c>
-      <c r="EC15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="ED15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="EE15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="EF15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="EG15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="EH15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="EI15" s="14" t="s">
-        <v>2269</v>
-      </c>
-      <c r="EJ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="EK15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="EL15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="EM15" s="14" t="s">
-        <v>2296</v>
-      </c>
-      <c r="EN15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="EO15" s="14" t="s">
-        <v>2267</v>
-      </c>
-      <c r="EP15" s="14" t="s">
-        <v>2273</v>
-      </c>
-      <c r="EQ15" s="14" t="s">
-        <v>2293</v>
-      </c>
-      <c r="ER15" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="ES15" s="14" t="s">
-        <v>2255</v>
-      </c>
-      <c r="ET15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="EU15" s="14" t="s">
-        <v>2271</v>
-      </c>
-      <c r="EV15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="EW15" s="14" t="s">
+      <c r="FK15" s="14" t="s">
         <v>2264</v>
       </c>
-      <c r="EX15" s="14" t="s">
-        <v>2271</v>
-      </c>
-      <c r="EY15" s="14" t="s">
-        <v>2274</v>
-      </c>
-      <c r="EZ15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="FA15" s="14" t="s">
-        <v>2267</v>
-      </c>
-      <c r="FB15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="FC15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="FD15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="FE15" s="14" t="s">
-        <v>2266</v>
-      </c>
-      <c r="FF15" s="14" t="s">
-        <v>2257</v>
-      </c>
-      <c r="FG15" s="14" t="s">
-        <v>2298</v>
-      </c>
-      <c r="FH15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="FI15" s="14" t="s">
-        <v>2277</v>
-      </c>
-      <c r="FJ15" s="14" t="s">
-        <v>2271</v>
-      </c>
-      <c r="FK15" s="14" t="s">
-        <v>2266</v>
-      </c>
       <c r="FL15" s="14" t="s">
-        <v>2262</v>
+        <v>2260</v>
       </c>
       <c r="FM15" s="14" t="s">
-        <v>2277</v>
+        <v>2275</v>
       </c>
       <c r="FN15" s="5"/>
       <c r="FO15" s="5"/>
@@ -18697,513 +18697,513 @@
       <c r="GN15" s="5"/>
       <c r="GO15" s="5"/>
     </row>
-    <row r="16" spans="1:197" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:197" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>2214</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>2256</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="D16" s="14" t="s">
         <v>2258</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>2260</v>
-      </c>
       <c r="E16" s="14" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="F16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>2263</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>2265</v>
-      </c>
       <c r="H16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>2261</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="N16" s="14" t="s">
         <v>2263</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="L16" s="33" t="s">
-        <v>2263</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>2265</v>
-      </c>
       <c r="O16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>2272</v>
+        <v>2270</v>
       </c>
       <c r="Q16" s="14" t="s">
+        <v>2266</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>2266</v>
+      </c>
+      <c r="S16" s="14" t="s">
         <v>2268</v>
       </c>
-      <c r="R16" s="14" t="s">
-        <v>2268</v>
-      </c>
-      <c r="S16" s="14" t="s">
+      <c r="T16" s="46" t="s">
+        <v>2266</v>
+      </c>
+      <c r="U16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="V16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="X16" s="14" t="s">
         <v>2270</v>
       </c>
-      <c r="T16" s="46" t="s">
-        <v>2268</v>
-      </c>
-      <c r="U16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="V16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="W16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="X16" s="14" t="s">
-        <v>2272</v>
-      </c>
       <c r="Y16" s="14" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="Z16" s="14" t="s">
-        <v>2275</v>
+        <v>2273</v>
       </c>
       <c r="AA16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AB16" s="14" t="s">
-        <v>2268</v>
+        <v>2266</v>
       </c>
       <c r="AC16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AD16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AE16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AF16" s="14" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="AG16" s="14" t="s">
-        <v>2272</v>
+        <v>2270</v>
       </c>
       <c r="AH16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AI16" s="14" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="AJ16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AK16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AL16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AM16" s="14" t="s">
-        <v>2282</v>
+        <v>2280</v>
       </c>
       <c r="AN16" s="14" t="s">
-        <v>2283</v>
+        <v>2281</v>
       </c>
       <c r="AO16" s="14" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="AP16" s="14" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="AQ16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AR16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AS16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AT16" s="14" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="AU16" s="14" t="s">
         <v>1128</v>
       </c>
       <c r="AV16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="AW16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="AX16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="AY16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="AZ16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BA16" s="14" t="s">
+        <v>2273</v>
+      </c>
+      <c r="BB16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="BC16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BD16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="BE16" s="14" t="s">
+        <v>2280</v>
+      </c>
+      <c r="BF16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BG16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BH16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="BI16" s="14" t="s">
+        <v>2284</v>
+      </c>
+      <c r="BJ16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="BK16" s="14" t="s">
+        <v>2281</v>
+      </c>
+      <c r="BL16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BM16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="BN16" s="14" t="s">
+        <v>2256</v>
+      </c>
+      <c r="BO16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BP16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BQ16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BR16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="BS16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BT16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BU16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BV16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BW16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="BX16" s="14" t="s">
+        <v>2286</v>
+      </c>
+      <c r="BY16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="BZ16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CA16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CB16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="CC16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="CD16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CE16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="CF16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CG16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="CH16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CI16" s="14" t="s">
+        <v>2256</v>
+      </c>
+      <c r="CJ16" s="14" t="s">
+        <v>2287</v>
+      </c>
+      <c r="CK16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CL16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CM16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CN16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CO16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="CP16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CQ16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="CR16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="CS16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CT16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="CU16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="CV16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CW16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CX16" s="14" t="s">
+        <v>2287</v>
+      </c>
+      <c r="CY16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CZ16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DA16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DB16" s="14" t="s">
+        <v>2273</v>
+      </c>
+      <c r="DC16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DD16" s="14" t="s">
+        <v>2266</v>
+      </c>
+      <c r="DE16" s="14" t="s">
+        <v>2292</v>
+      </c>
+      <c r="DF16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="DG16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DH16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DI16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="DJ16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="DK16" s="33" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DL16" s="14" t="s">
+        <v>2258</v>
+      </c>
+      <c r="DM16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="DN16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DO16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="DP16" s="14" t="s">
+        <v>2256</v>
+      </c>
+      <c r="DQ16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DR16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DS16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="DT16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DU16" s="14" t="s">
+        <v>2287</v>
+      </c>
+      <c r="DV16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DW16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="DX16" s="14" t="s">
+        <v>2256</v>
+      </c>
+      <c r="DY16" s="14" t="s">
+        <v>2281</v>
+      </c>
+      <c r="DZ16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="EA16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EB16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="EC16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="ED16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EE16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EF16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EG16" s="14" t="s">
+        <v>2281</v>
+      </c>
+      <c r="EH16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="EI16" s="14" t="s">
+        <v>2268</v>
+      </c>
+      <c r="EJ16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EK16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="EL16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EM16" s="14" t="s">
         <v>2263</v>
       </c>
-      <c r="AW16" s="14" t="s">
+      <c r="EN16" s="14" t="s">
+        <v>2281</v>
+      </c>
+      <c r="EO16" s="14" t="s">
+        <v>2266</v>
+      </c>
+      <c r="EP16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="EQ16" s="14" t="s">
+        <v>2292</v>
+      </c>
+      <c r="ER16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="ES16" s="14" t="s">
+        <v>2254</v>
+      </c>
+      <c r="ET16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EU16" s="14" t="s">
+        <v>2295</v>
+      </c>
+      <c r="EV16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EW16" s="14" t="s">
         <v>2263</v>
       </c>
-      <c r="AX16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="AY16" s="14" t="s">
+      <c r="EX16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="EY16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="EZ16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="FA16" s="14" t="s">
+        <v>2292</v>
+      </c>
+      <c r="FB16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="FC16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="FD16" s="14" t="s">
+        <v>2270</v>
+      </c>
+      <c r="FE16" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="FF16" s="14" t="s">
         <v>2256</v>
       </c>
-      <c r="AZ16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BA16" s="14" t="s">
-        <v>2275</v>
-      </c>
-      <c r="BB16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="BC16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BD16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="BE16" s="14" t="s">
-        <v>2282</v>
-      </c>
-      <c r="BF16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BG16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BH16" s="14" t="s">
+      <c r="FG16" s="2" t="s">
+        <v>2261</v>
+      </c>
+      <c r="FH16" s="2" t="s">
         <v>2270</v>
       </c>
-      <c r="BI16" s="14" t="s">
-        <v>2286</v>
-      </c>
-      <c r="BJ16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="BK16" s="14" t="s">
-        <v>2283</v>
-      </c>
-      <c r="BL16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BM16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="BN16" s="14" t="s">
-        <v>2258</v>
-      </c>
-      <c r="BO16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BP16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BQ16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BR16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="BS16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BT16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BU16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BV16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BW16" s="14" t="s">
+      <c r="FI16" s="2" t="s">
+        <v>2254</v>
+      </c>
+      <c r="FJ16" s="2" t="s">
+        <v>2295</v>
+      </c>
+      <c r="FK16" s="2" t="s">
+        <v>2261</v>
+      </c>
+      <c r="FL16" s="2" t="s">
+        <v>2281</v>
+      </c>
+      <c r="FM16" s="2" t="s">
         <v>2270</v>
-      </c>
-      <c r="BX16" s="14" t="s">
-        <v>2288</v>
-      </c>
-      <c r="BY16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="BZ16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CA16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CB16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="CC16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="CD16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CE16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="CF16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CG16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="CH16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CI16" s="14" t="s">
-        <v>2258</v>
-      </c>
-      <c r="CJ16" s="14" t="s">
-        <v>2289</v>
-      </c>
-      <c r="CK16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CL16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CM16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CN16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CO16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="CP16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CQ16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="CR16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="CS16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CT16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="CU16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="CV16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CW16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CX16" s="14" t="s">
-        <v>2289</v>
-      </c>
-      <c r="CY16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="CZ16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DA16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DB16" s="14" t="s">
-        <v>2275</v>
-      </c>
-      <c r="DC16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DD16" s="14" t="s">
-        <v>2268</v>
-      </c>
-      <c r="DE16" s="14" t="s">
-        <v>2294</v>
-      </c>
-      <c r="DF16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="DG16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DH16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DI16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="DJ16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="DK16" s="33" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DL16" s="14" t="s">
-        <v>2260</v>
-      </c>
-      <c r="DM16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="DN16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DO16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="DP16" s="14" t="s">
-        <v>2258</v>
-      </c>
-      <c r="DQ16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DR16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DS16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="DT16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DU16" s="14" t="s">
-        <v>2289</v>
-      </c>
-      <c r="DV16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DW16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="DX16" s="14" t="s">
-        <v>2258</v>
-      </c>
-      <c r="DY16" s="14" t="s">
-        <v>2283</v>
-      </c>
-      <c r="DZ16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="EA16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EB16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="EC16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="ED16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EE16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EF16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EG16" s="14" t="s">
-        <v>2283</v>
-      </c>
-      <c r="EH16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="EI16" s="14" t="s">
-        <v>2270</v>
-      </c>
-      <c r="EJ16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EK16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="EL16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EM16" s="14" t="s">
-        <v>2265</v>
-      </c>
-      <c r="EN16" s="14" t="s">
-        <v>2283</v>
-      </c>
-      <c r="EO16" s="14" t="s">
-        <v>2268</v>
-      </c>
-      <c r="EP16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="EQ16" s="14" t="s">
-        <v>2294</v>
-      </c>
-      <c r="ER16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="ES16" s="14" t="s">
-        <v>2256</v>
-      </c>
-      <c r="ET16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EU16" s="14" t="s">
-        <v>2297</v>
-      </c>
-      <c r="EV16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EW16" s="14" t="s">
-        <v>2265</v>
-      </c>
-      <c r="EX16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="EY16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="EZ16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="FA16" s="14" t="s">
-        <v>2294</v>
-      </c>
-      <c r="FB16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="FC16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="FD16" s="14" t="s">
-        <v>2272</v>
-      </c>
-      <c r="FE16" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="FF16" s="14" t="s">
-        <v>2258</v>
-      </c>
-      <c r="FG16" s="2" t="s">
-        <v>2263</v>
-      </c>
-      <c r="FH16" s="2" t="s">
-        <v>2272</v>
-      </c>
-      <c r="FI16" s="2" t="s">
-        <v>2256</v>
-      </c>
-      <c r="FJ16" s="2" t="s">
-        <v>2297</v>
-      </c>
-      <c r="FK16" s="2" t="s">
-        <v>2263</v>
-      </c>
-      <c r="FL16" s="2" t="s">
-        <v>2283</v>
-      </c>
-      <c r="FM16" s="2" t="s">
-        <v>2272</v>
       </c>
       <c r="FN16" s="5"/>
       <c r="FO16" s="5"/>
@@ -19234,9 +19234,9 @@
       <c r="GN16" s="5"/>
       <c r="GO16" s="5"/>
     </row>
-    <row r="17" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>630</v>
@@ -19771,9 +19771,9 @@
       <c r="GN17" s="2"/>
       <c r="GO17" s="2"/>
     </row>
-    <row r="18" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>714</v>
@@ -19782,7 +19782,7 @@
         <v>719</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>1261</v>
@@ -19803,7 +19803,7 @@
         <v>748</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>1208</v>
@@ -19815,7 +19815,7 @@
         <v>758</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>2334</v>
+        <v>2332</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>1311</v>
@@ -19905,13 +19905,13 @@
         <v>1449</v>
       </c>
       <c r="AS18" s="2" t="s">
-        <v>2312</v>
+        <v>2310</v>
       </c>
       <c r="AT18" s="2" t="s">
         <v>1574</v>
       </c>
       <c r="AU18" s="2" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="AV18" s="2" t="s">
         <v>644</v>
@@ -19923,7 +19923,7 @@
         <v>809</v>
       </c>
       <c r="AY18" s="2" t="s">
-        <v>2335</v>
+        <v>2333</v>
       </c>
       <c r="AZ18" s="2" t="s">
         <v>812</v>
@@ -20001,7 +20001,7 @@
         <v>856</v>
       </c>
       <c r="BY18" s="2" t="s">
-        <v>2332</v>
+        <v>2330</v>
       </c>
       <c r="BZ18" s="2" t="s">
         <v>861</v>
@@ -20178,7 +20178,7 @@
         <v>1026</v>
       </c>
       <c r="EF18" s="2" t="s">
-        <v>2361</v>
+        <v>2359</v>
       </c>
       <c r="EG18" s="3" t="s">
         <v>1869</v>
@@ -20241,7 +20241,7 @@
         <v>1098</v>
       </c>
       <c r="FA18" s="2" t="s">
-        <v>2336</v>
+        <v>2334</v>
       </c>
       <c r="FB18" s="2" t="s">
         <v>1106</v>
@@ -20259,13 +20259,13 @@
         <v>1840</v>
       </c>
       <c r="FG18" s="2" t="s">
-        <v>2299</v>
+        <v>2297</v>
       </c>
       <c r="FH18" s="2" t="s">
         <v>1127</v>
       </c>
       <c r="FI18" s="2" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
       <c r="FJ18" s="2" t="s">
         <v>1134</v>
@@ -20308,9 +20308,9 @@
       <c r="GN18" s="2"/>
       <c r="GO18" s="2"/>
     </row>
-    <row r="19" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>398</v>
@@ -20785,9 +20785,9 @@
       <c r="GN19" s="11"/>
       <c r="GO19" s="11"/>
     </row>
-    <row r="20" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>398</v>
@@ -21190,7 +21190,7 @@
         <v>398</v>
       </c>
       <c r="EX20" s="11" t="s">
-        <v>2426</v>
+        <v>2424</v>
       </c>
       <c r="EY20" s="43" t="s">
         <v>1403</v>
@@ -21262,9 +21262,9 @@
       <c r="GN20" s="43"/>
       <c r="GO20" s="43"/>
     </row>
-    <row r="21" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="13" t="s">
@@ -21366,7 +21366,7 @@
         <v>1688</v>
       </c>
       <c r="AM21" s="2" t="s">
-        <v>2313</v>
+        <v>2311</v>
       </c>
       <c r="AN21" s="4"/>
       <c r="AO21" s="2" t="s">
@@ -21380,7 +21380,7 @@
         <v>1450</v>
       </c>
       <c r="AS21" s="2" t="s">
-        <v>2318</v>
+        <v>2316</v>
       </c>
       <c r="AT21" s="2" t="s">
         <v>1575</v>
@@ -21415,7 +21415,7 @@
         <v>1631</v>
       </c>
       <c r="BF21" s="3" t="s">
-        <v>2307</v>
+        <v>2305</v>
       </c>
       <c r="BG21" s="3" t="s">
         <v>1637</v>
@@ -21576,7 +21576,7 @@
         <v>1904</v>
       </c>
       <c r="DT21" s="2" t="s">
-        <v>2319</v>
+        <v>2317</v>
       </c>
       <c r="DU21" s="11" t="s">
         <v>398</v>
@@ -21728,9 +21728,9 @@
       <c r="GN21" s="2"/>
       <c r="GO21" s="2"/>
     </row>
-    <row r="22" spans="1:197" s="37" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:197" s="37" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>2281</v>
+        <v>2279</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>1143</v>
@@ -22265,9 +22265,9 @@
       <c r="GN22" s="5"/>
       <c r="GO22" s="5"/>
     </row>
-    <row r="23" spans="1:197" s="37" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:197" s="37" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>1136</v>
@@ -22802,9 +22802,9 @@
       <c r="GN23" s="5"/>
       <c r="GO23" s="5"/>
     </row>
-    <row r="24" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>2231</v>
+        <v>2229</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>195</v>
@@ -23339,9 +23339,9 @@
       <c r="GN24" s="2"/>
       <c r="GO24" s="2"/>
     </row>
-    <row r="25" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>713</v>
@@ -23353,7 +23353,7 @@
         <v>720</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>2437</v>
+        <v>2435</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>725</v>
@@ -23371,7 +23371,7 @@
         <v>756</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="L25" s="11" t="s">
         <v>750</v>
@@ -23383,10 +23383,10 @@
         <v>759</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>2333</v>
+        <v>2331</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>2438</v>
+        <v>2436</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>760</v>
@@ -23398,7 +23398,7 @@
         <v>1570</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>2439</v>
+        <v>2437</v>
       </c>
       <c r="U25" s="2" t="s">
         <v>763</v>
@@ -23473,7 +23473,7 @@
         <v>803</v>
       </c>
       <c r="AS25" s="14" t="s">
-        <v>2320</v>
+        <v>2318</v>
       </c>
       <c r="AT25" s="2" t="s">
         <v>1576</v>
@@ -23509,7 +23509,7 @@
         <v>819</v>
       </c>
       <c r="BE25" s="11" t="s">
-        <v>2440</v>
+        <v>2438</v>
       </c>
       <c r="BF25" s="3" t="s">
         <v>1632</v>
@@ -23536,7 +23536,7 @@
         <v>832</v>
       </c>
       <c r="BN25" s="11" t="s">
-        <v>2441</v>
+        <v>2439</v>
       </c>
       <c r="BO25" s="11" t="s">
         <v>835</v>
@@ -23581,7 +23581,7 @@
         <v>869</v>
       </c>
       <c r="CC25" s="2" t="s">
-        <v>2442</v>
+        <v>2440</v>
       </c>
       <c r="CD25" s="11" t="s">
         <v>872</v>
@@ -23632,7 +23632,7 @@
         <v>911</v>
       </c>
       <c r="CT25" s="11" t="s">
-        <v>2442</v>
+        <v>2440</v>
       </c>
       <c r="CU25" s="11" t="s">
         <v>634</v>
@@ -23674,7 +23674,7 @@
         <v>959</v>
       </c>
       <c r="DH25" s="11" t="s">
-        <v>2442</v>
+        <v>2440</v>
       </c>
       <c r="DI25" s="11" t="s">
         <v>1438</v>
@@ -23698,10 +23698,10 @@
         <v>1361</v>
       </c>
       <c r="DP25" s="11" t="s">
-        <v>2443</v>
+        <v>2441</v>
       </c>
       <c r="DQ25" s="11" t="s">
-        <v>2442</v>
+        <v>2440</v>
       </c>
       <c r="DR25" s="11" t="s">
         <v>983</v>
@@ -23761,10 +23761,10 @@
         <v>1045</v>
       </c>
       <c r="EK25" s="11" t="s">
-        <v>2444</v>
+        <v>2442</v>
       </c>
       <c r="EL25" s="11" t="s">
-        <v>2444</v>
+        <v>2442</v>
       </c>
       <c r="EM25" s="2" t="s">
         <v>1050</v>
@@ -23876,9 +23876,9 @@
       <c r="GN25" s="2"/>
       <c r="GO25" s="2"/>
     </row>
-    <row r="26" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>2233</v>
+        <v>2231</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>398</v>
@@ -24222,7 +24222,7 @@
         <v>1100</v>
       </c>
       <c r="FA26" s="2" t="s">
-        <v>2569</v>
+        <v>2567</v>
       </c>
       <c r="FB26" s="2" t="s">
         <v>1108</v>
@@ -24281,7 +24281,7 @@
       <c r="GN26" s="2"/>
       <c r="GO26" s="2"/>
     </row>
-    <row r="27" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>742</v>
       </c>
@@ -24622,7 +24622,7 @@
         <v>398</v>
       </c>
       <c r="DT27" s="2" t="s">
-        <v>2314</v>
+        <v>2312</v>
       </c>
       <c r="DU27" s="4"/>
       <c r="DV27" s="2" t="s">
@@ -24776,9 +24776,9 @@
       <c r="GN27" s="2"/>
       <c r="GO27" s="2"/>
     </row>
-    <row r="28" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>2471</v>
+        <v>2469</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>594</v>
@@ -24799,13 +24799,13 @@
         <v>594</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>594</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>398</v>
@@ -24825,7 +24825,7 @@
         <v>594</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>398</v>
@@ -24834,7 +24834,7 @@
         <v>398</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="V28" s="2" t="s">
         <v>594</v>
@@ -24849,10 +24849,10 @@
         <v>594</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AB28" s="11" t="s">
         <v>398</v>
@@ -24864,7 +24864,7 @@
         <v>594</v>
       </c>
       <c r="AE28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AF28" s="2" t="s">
         <v>594</v>
@@ -24873,10 +24873,10 @@
         <v>398</v>
       </c>
       <c r="AH28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AI28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AJ28" s="11" t="s">
         <v>398</v>
@@ -24889,7 +24889,7 @@
       </c>
       <c r="AM28" s="4"/>
       <c r="AN28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AO28" s="2" t="s">
         <v>594</v>
@@ -24901,7 +24901,7 @@
         <v>594</v>
       </c>
       <c r="AR28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AS28" s="2" t="s">
         <v>594</v>
@@ -24913,20 +24913,20 @@
         <v>398</v>
       </c>
       <c r="AV28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AW28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AX28" s="11" t="s">
         <v>398</v>
       </c>
       <c r="AY28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="AZ28" s="4"/>
       <c r="BA28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="BB28" s="2" t="s">
         <v>594</v>
@@ -24935,7 +24935,7 @@
         <v>594</v>
       </c>
       <c r="BD28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="BE28" s="11" t="s">
         <v>398</v>
@@ -24959,7 +24959,7 @@
         <v>594</v>
       </c>
       <c r="BL28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="BM28" s="2" t="s">
         <v>594</v>
@@ -24979,7 +24979,7 @@
         <v>398</v>
       </c>
       <c r="BT28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="BU28" s="2" t="s">
         <v>594</v>
@@ -25007,7 +25007,7 @@
         <v>398</v>
       </c>
       <c r="CD28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="CE28" s="11" t="s">
         <v>398</v>
@@ -25032,10 +25032,10 @@
         <v>594</v>
       </c>
       <c r="CM28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="CN28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="CO28" s="2" t="s">
         <v>594</v>
@@ -25044,7 +25044,7 @@
         <v>594</v>
       </c>
       <c r="CQ28" s="2" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="CR28" s="2" t="s">
         <v>594</v>
@@ -25065,7 +25065,7 @@
       </c>
       <c r="CY28" s="4"/>
       <c r="CZ28" s="2" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="DA28" s="2" t="s">
         <v>594</v>
@@ -25080,11 +25080,11 @@
         <v>398</v>
       </c>
       <c r="DE28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="DF28" s="2"/>
       <c r="DG28" s="2" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="DH28" s="4"/>
       <c r="DI28" s="11" t="s">
@@ -25094,7 +25094,7 @@
         <v>398</v>
       </c>
       <c r="DK28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="DL28" s="11" t="s">
         <v>398</v>
@@ -25121,10 +25121,10 @@
       </c>
       <c r="DU28" s="4"/>
       <c r="DV28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="DW28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="DX28" s="11" t="s">
         <v>398</v>
@@ -25140,7 +25140,7 @@
         <v>594</v>
       </c>
       <c r="EC28" s="2" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="ED28" s="2" t="s">
         <v>594</v>
@@ -25162,19 +25162,19 @@
         <v>398</v>
       </c>
       <c r="EM28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="EN28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="EO28" s="2" t="s">
         <v>594</v>
       </c>
       <c r="EP28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="EQ28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="ER28" s="3" t="s">
         <v>398</v>
@@ -25183,11 +25183,11 @@
         <v>398</v>
       </c>
       <c r="ET28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="EU28" s="2"/>
       <c r="EV28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="EW28" s="2" t="s">
         <v>594</v>
@@ -25199,24 +25199,24 @@
         <v>398</v>
       </c>
       <c r="EZ28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="FA28" s="2" t="s">
         <v>594</v>
       </c>
       <c r="FB28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="FC28" s="2" t="s">
         <v>594</v>
       </c>
       <c r="FD28" s="2"/>
       <c r="FE28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="FF28" s="4"/>
       <c r="FG28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="FH28" s="3" t="s">
         <v>398</v>
@@ -25228,7 +25228,7 @@
         <v>594</v>
       </c>
       <c r="FK28" s="2" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="FL28" s="2" t="s">
         <v>594</v>
@@ -25265,7 +25265,7 @@
       <c r="GN28" s="2"/>
       <c r="GO28" s="2"/>
     </row>
-    <row r="29" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>743</v>
       </c>
@@ -25393,7 +25393,7 @@
         <v>804</v>
       </c>
       <c r="AS29" s="14" t="s">
-        <v>2472</v>
+        <v>2470</v>
       </c>
       <c r="AT29" s="11" t="s">
         <v>398</v>
@@ -25606,7 +25606,7 @@
         <v>398</v>
       </c>
       <c r="DT29" s="2" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
       <c r="DU29" s="4"/>
       <c r="DV29" s="2" t="s">
@@ -25679,7 +25679,7 @@
         <v>968</v>
       </c>
       <c r="EW29" s="2" t="s">
-        <v>2473</v>
+        <v>2471</v>
       </c>
       <c r="EX29" s="2" t="s">
         <v>398</v>
@@ -25754,9 +25754,9 @@
       <c r="GN29" s="2"/>
       <c r="GO29" s="2"/>
     </row>
-    <row r="30" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>2234</v>
+        <v>2232</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>669</v>
@@ -26241,25 +26241,25 @@
       <c r="GN30" s="2"/>
       <c r="GO30" s="2"/>
     </row>
-    <row r="31" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>2337</v>
+        <v>2335</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>2341</v>
+        <v>2339</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="30" t="s">
-        <v>2378</v>
+        <v>2376</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>398</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>2382</v>
+        <v>2380</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>2383</v>
+        <v>2381</v>
       </c>
       <c r="H31" s="30" t="s">
         <v>2163</v>
@@ -26269,32 +26269,32 @@
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="14" t="s">
-        <v>2342</v>
+        <v>2340</v>
       </c>
       <c r="L31" s="14" t="s">
-        <v>2338</v>
+        <v>2336</v>
       </c>
       <c r="M31" s="14" t="s">
         <v>2161</v>
       </c>
       <c r="N31" s="30" t="s">
-        <v>2384</v>
+        <v>2382</v>
       </c>
       <c r="O31" s="30" t="s">
         <v>2160</v>
       </c>
       <c r="P31" s="23"/>
       <c r="Q31" s="30" t="s">
-        <v>2408</v>
+        <v>2406</v>
       </c>
       <c r="R31" s="30" t="s">
         <v>2159</v>
       </c>
       <c r="S31" s="30" t="s">
-        <v>2344</v>
+        <v>2342</v>
       </c>
       <c r="U31" s="30" t="s">
-        <v>2343</v>
+        <v>2341</v>
       </c>
       <c r="V31" s="23"/>
       <c r="W31" s="30" t="s">
@@ -26307,7 +26307,7 @@
         <v>2156</v>
       </c>
       <c r="Z31" s="14" t="s">
-        <v>2386</v>
+        <v>2384</v>
       </c>
       <c r="AA31" s="30" t="s">
         <v>2155</v>
@@ -26316,13 +26316,13 @@
         <v>2154</v>
       </c>
       <c r="AC31" s="30" t="s">
-        <v>2345</v>
+        <v>2343</v>
       </c>
       <c r="AD31" s="30" t="s">
         <v>2153</v>
       </c>
       <c r="AE31" s="14" t="s">
-        <v>2387</v>
+        <v>2385</v>
       </c>
       <c r="AF31" s="30" t="s">
         <v>2152</v>
@@ -26339,14 +26339,14 @@
         <v>2149</v>
       </c>
       <c r="AL31" s="30" t="s">
-        <v>2346</v>
+        <v>2344</v>
       </c>
       <c r="AM31" s="30" t="s">
-        <v>2389</v>
+        <v>2387</v>
       </c>
       <c r="AN31" s="23"/>
       <c r="AO31" s="14" t="s">
-        <v>2347</v>
+        <v>2345</v>
       </c>
       <c r="AP31" s="14" t="s">
         <v>2148</v>
@@ -26356,24 +26356,24 @@
         <v>398</v>
       </c>
       <c r="AS31" s="30" t="s">
-        <v>2418</v>
+        <v>2416</v>
       </c>
       <c r="AU31" s="30" t="s">
-        <v>2377</v>
+        <v>2375</v>
       </c>
       <c r="AV31" s="30" t="s">
-        <v>2419</v>
+        <v>2417</v>
       </c>
       <c r="AW31" s="23"/>
       <c r="AX31" s="23"/>
       <c r="AY31" s="14" t="s">
-        <v>2348</v>
+        <v>2346</v>
       </c>
       <c r="AZ31" s="30" t="s">
-        <v>2409</v>
+        <v>2407</v>
       </c>
       <c r="BA31" s="14" t="s">
-        <v>2349</v>
+        <v>2347</v>
       </c>
       <c r="BB31" s="14" t="s">
         <v>2147</v>
@@ -26382,20 +26382,20 @@
         <v>2146</v>
       </c>
       <c r="BD31" s="30" t="s">
-        <v>2393</v>
+        <v>2391</v>
       </c>
       <c r="BE31" s="30" t="s">
         <v>2145</v>
       </c>
       <c r="BF31" s="23"/>
       <c r="BG31" s="30" t="s">
-        <v>2350</v>
+        <v>2348</v>
       </c>
       <c r="BH31" s="14" t="s">
         <v>2144</v>
       </c>
       <c r="BI31" s="30" t="s">
-        <v>2448</v>
+        <v>2446</v>
       </c>
       <c r="BJ31" s="30" t="s">
         <v>2143</v>
@@ -26404,7 +26404,7 @@
         <v>2142</v>
       </c>
       <c r="BL31" s="30" t="s">
-        <v>2339</v>
+        <v>2337</v>
       </c>
       <c r="BM31" s="30" t="s">
         <v>2141</v>
@@ -26419,7 +26419,7 @@
       </c>
       <c r="BR31" s="23"/>
       <c r="BS31" s="30" t="s">
-        <v>2359</v>
+        <v>2357</v>
       </c>
       <c r="BT31" s="14" t="s">
         <v>2140</v>
@@ -26429,16 +26429,16 @@
       </c>
       <c r="BV31" s="26"/>
       <c r="BW31" s="30" t="s">
-        <v>2410</v>
+        <v>2408</v>
       </c>
       <c r="BX31" s="30" t="s">
         <v>2138</v>
       </c>
       <c r="BY31" s="30" t="s">
-        <v>2394</v>
+        <v>2392</v>
       </c>
       <c r="BZ31" s="30" t="s">
-        <v>2395</v>
+        <v>2393</v>
       </c>
       <c r="CA31" s="30" t="s">
         <v>2137</v>
@@ -26488,23 +26488,23 @@
       </c>
       <c r="CR31" s="23"/>
       <c r="CS31" s="30" t="s">
-        <v>2412</v>
+        <v>2410</v>
       </c>
       <c r="CT31" s="23"/>
       <c r="CU31" s="30" t="s">
-        <v>2351</v>
+        <v>2349</v>
       </c>
       <c r="CV31" s="30" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
       <c r="CW31" s="24" t="s">
         <v>2123</v>
       </c>
       <c r="CX31" s="30" t="s">
-        <v>2411</v>
+        <v>2409</v>
       </c>
       <c r="CY31" s="30" t="s">
-        <v>2458</v>
+        <v>2456</v>
       </c>
       <c r="CZ31" s="30" t="s">
         <v>2122</v>
@@ -26514,20 +26514,20 @@
       </c>
       <c r="DB31" s="23"/>
       <c r="DC31" s="30" t="s">
+        <v>2395</v>
+      </c>
+      <c r="DD31" s="30" t="s">
+        <v>2396</v>
+      </c>
+      <c r="DE31" s="30" t="s">
         <v>2397</v>
-      </c>
-      <c r="DD31" s="30" t="s">
-        <v>2398</v>
-      </c>
-      <c r="DE31" s="30" t="s">
-        <v>2399</v>
       </c>
       <c r="DF31" s="23"/>
       <c r="DG31" s="14" t="s">
         <v>2120</v>
       </c>
       <c r="DH31" s="30" t="s">
-        <v>2413</v>
+        <v>2411</v>
       </c>
       <c r="DI31" s="23"/>
       <c r="DJ31" s="14" t="s">
@@ -26569,20 +26569,20 @@
       <c r="DY31" s="23"/>
       <c r="DZ31" s="23"/>
       <c r="EA31" s="30" t="s">
-        <v>2400</v>
+        <v>2398</v>
       </c>
       <c r="EB31" s="30" t="s">
-        <v>2414</v>
+        <v>2412</v>
       </c>
       <c r="EC31" s="13"/>
       <c r="ED31" s="30" t="s">
-        <v>2353</v>
+        <v>2351</v>
       </c>
       <c r="EE31" s="14" t="s">
         <v>2112</v>
       </c>
       <c r="EF31" s="30" t="s">
-        <v>2362</v>
+        <v>2360</v>
       </c>
       <c r="EG31" s="23"/>
       <c r="EH31" s="23"/>
@@ -26595,13 +26595,13 @@
         <v>2110</v>
       </c>
       <c r="EM31" s="30" t="s">
-        <v>2401</v>
+        <v>2399</v>
       </c>
       <c r="EN31" s="30" t="s">
-        <v>2425</v>
+        <v>2423</v>
       </c>
       <c r="EO31" s="30" t="s">
-        <v>2354</v>
+        <v>2352</v>
       </c>
       <c r="EP31" s="30" t="s">
         <v>2109</v>
@@ -26619,36 +26619,36 @@
         <v>2105</v>
       </c>
       <c r="EU31" s="30" t="s">
-        <v>2402</v>
+        <v>2400</v>
       </c>
       <c r="EV31" s="30" t="s">
         <v>2104</v>
       </c>
       <c r="EW31" s="23"/>
       <c r="EX31" s="14" t="s">
-        <v>2403</v>
+        <v>2401</v>
       </c>
       <c r="EY31" s="14" t="s">
         <v>2103</v>
       </c>
       <c r="EZ31" s="14" t="s">
-        <v>2355</v>
+        <v>2353</v>
       </c>
       <c r="FA31" s="30" t="s">
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="FB31" s="30" t="s">
-        <v>2405</v>
+        <v>2403</v>
       </c>
       <c r="FC31" s="30" t="s">
-        <v>2365</v>
+        <v>2363</v>
       </c>
       <c r="FE31" s="30" t="s">
         <v>2102</v>
       </c>
       <c r="FF31" s="23"/>
       <c r="FG31" s="30" t="s">
-        <v>2406</v>
+        <v>2404</v>
       </c>
       <c r="FI31" s="30" t="s">
         <v>2101</v>
@@ -26748,9 +26748,9 @@
         <v>398</v>
       </c>
     </row>
-    <row r="32" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>2235</v>
+        <v>2233</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>716</v>
@@ -26759,14 +26759,14 @@
         <v>1255</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>2379</v>
+        <v>2377</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="28" t="s">
-        <v>2381</v>
+        <v>2379</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="36" t="s">
@@ -26774,21 +26774,21 @@
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="28" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
       <c r="L32" s="28" t="s">
         <v>1209</v>
       </c>
       <c r="M32" s="13"/>
       <c r="N32" s="28" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
       <c r="O32" s="28" t="s">
         <v>1283</v>
       </c>
       <c r="P32" s="13"/>
       <c r="Q32" s="28" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
       <c r="R32" s="13"/>
       <c r="S32" s="28" t="s">
@@ -26810,16 +26810,16 @@
         <v>780</v>
       </c>
       <c r="AB32" s="28" t="s">
-        <v>2417</v>
+        <v>2415</v>
       </c>
       <c r="AC32" s="28" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
       <c r="AD32" s="36" t="s">
         <v>1233</v>
       </c>
       <c r="AE32" s="28" t="s">
-        <v>2388</v>
+        <v>2386</v>
       </c>
       <c r="AF32" s="13"/>
       <c r="AG32" s="13"/>
@@ -26842,7 +26842,7 @@
         <v>398</v>
       </c>
       <c r="AS32" s="28" t="s">
-        <v>2321</v>
+        <v>2319</v>
       </c>
       <c r="AT32" s="28" t="s">
         <v>1579</v>
@@ -26857,7 +26857,7 @@
       </c>
       <c r="AY32" s="13"/>
       <c r="AZ32" s="28" t="s">
-        <v>2390</v>
+        <v>2388</v>
       </c>
       <c r="BA32" s="28" t="s">
         <v>1507</v>
@@ -26951,7 +26951,7 @@
       <c r="CP32" s="13"/>
       <c r="CQ32" s="13"/>
       <c r="CR32" s="28" t="s">
-        <v>2396</v>
+        <v>2394</v>
       </c>
       <c r="CS32" s="13"/>
       <c r="CT32" s="13"/>
@@ -26968,7 +26968,7 @@
         <v>1399</v>
       </c>
       <c r="DA32" s="28" t="s">
-        <v>2481</v>
+        <v>2479</v>
       </c>
       <c r="DB32" s="28" t="s">
         <v>1549</v>
@@ -27064,7 +27064,7 @@
         <v>1405</v>
       </c>
       <c r="EZ32" s="28" t="s">
-        <v>2482</v>
+        <v>2480</v>
       </c>
       <c r="FA32" s="13"/>
       <c r="FB32" s="13"/>
@@ -27083,7 +27083,7 @@
         <v>1524</v>
       </c>
       <c r="FI32" s="28" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="FJ32" s="28" t="s">
         <v>1672</v>
@@ -27092,7 +27092,7 @@
         <v>1189</v>
       </c>
       <c r="FL32" s="28" t="s">
-        <v>2484</v>
+        <v>2482</v>
       </c>
       <c r="FM32" s="28" t="s">
         <v>1566</v>
@@ -27126,7 +27126,7 @@
       <c r="GN32" s="3"/>
       <c r="GO32" s="3"/>
     </row>
-    <row r="33" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>704</v>
       </c>
@@ -27212,7 +27212,7 @@
       <c r="AQ33" s="4"/>
       <c r="AR33" s="4"/>
       <c r="AS33" s="14" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
       <c r="AT33" s="4"/>
       <c r="AU33" s="2" t="s">
@@ -27506,9 +27506,9 @@
       <c r="GN33" s="2"/>
       <c r="GO33" s="2"/>
     </row>
-    <row r="34" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>2236</v>
+        <v>2234</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -27567,7 +27567,7 @@
       <c r="AQ34" s="13"/>
       <c r="AR34" s="13"/>
       <c r="AS34" s="3" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
       <c r="AT34" s="13"/>
       <c r="AU34" s="13"/>
@@ -27769,9 +27769,9 @@
       <c r="GN34" s="3"/>
       <c r="GO34" s="3"/>
     </row>
-    <row r="35" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>2237</v>
+        <v>2235</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>710</v>
@@ -27901,7 +27901,7 @@
         <v>1051</v>
       </c>
       <c r="AS35" s="30" t="s">
-        <v>2315</v>
+        <v>2313</v>
       </c>
       <c r="AT35" s="3" t="s">
         <v>1578</v>
@@ -28300,9 +28300,9 @@
       <c r="GN35" s="3"/>
       <c r="GO35" s="3"/>
     </row>
-    <row r="36" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>2238</v>
+        <v>2236</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>398</v>
@@ -28835,9 +28835,9 @@
       <c r="GN36" s="3"/>
       <c r="GO36" s="3"/>
     </row>
-    <row r="37" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:197" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>2239</v>
+        <v>2237</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>398</v>
@@ -29368,15 +29368,15 @@
       <c r="GN37" s="3"/>
       <c r="GO37" s="3"/>
     </row>
-    <row r="38" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>2240</v>
+        <v>2238</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>2428</v>
+        <v>2426</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>2380</v>
+        <v>2378</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>2097</v>
@@ -29391,25 +29391,25 @@
         <v>2096</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>2368</v>
+        <v>2366</v>
       </c>
       <c r="I38" s="14" t="s">
         <v>2095</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>2243</v>
+        <v>2241</v>
       </c>
       <c r="K38" s="14" t="s">
         <v>2094</v>
       </c>
       <c r="L38" s="14" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>2245</v>
+        <v>2243</v>
       </c>
       <c r="N38" s="14" t="s">
-        <v>2244</v>
+        <v>2242</v>
       </c>
       <c r="O38" s="14" t="s">
         <v>2093</v>
@@ -29418,7 +29418,7 @@
         <v>1286</v>
       </c>
       <c r="Q38" s="14" t="s">
-        <v>2356</v>
+        <v>2354</v>
       </c>
       <c r="R38" s="14" t="s">
         <v>2092</v>
@@ -29430,13 +29430,13 @@
         <v>1286</v>
       </c>
       <c r="U38" s="14" t="s">
-        <v>2366</v>
+        <v>2364</v>
       </c>
       <c r="V38" s="25" t="s">
         <v>2091</v>
       </c>
       <c r="W38" s="25" t="s">
-        <v>2246</v>
+        <v>2244</v>
       </c>
       <c r="X38" s="40" t="s">
         <v>2090</v>
@@ -29454,7 +29454,7 @@
         <v>2086</v>
       </c>
       <c r="AC38" s="25" t="s">
-        <v>2430</v>
+        <v>2428</v>
       </c>
       <c r="AD38" s="14" t="s">
         <v>2085</v>
@@ -29466,37 +29466,37 @@
         <v>2083</v>
       </c>
       <c r="AG38" s="25" t="s">
-        <v>2303</v>
+        <v>2301</v>
       </c>
       <c r="AH38" s="44" t="s">
         <v>2082</v>
       </c>
       <c r="AI38" s="14" t="s">
-        <v>2446</v>
+        <v>2444</v>
       </c>
       <c r="AJ38" s="25" t="s">
         <v>2081</v>
       </c>
       <c r="AK38" s="14" t="s">
-        <v>2429</v>
+        <v>2427</v>
       </c>
       <c r="AL38" s="14" t="s">
         <v>2080</v>
       </c>
       <c r="AM38" s="25" t="s">
-        <v>2247</v>
+        <v>2245</v>
       </c>
       <c r="AN38" s="25" t="s">
         <v>2079</v>
       </c>
       <c r="AO38" s="25" t="s">
-        <v>2248</v>
+        <v>2246</v>
       </c>
       <c r="AP38" s="14" t="s">
         <v>2078</v>
       </c>
       <c r="AQ38" s="25" t="s">
-        <v>2249</v>
+        <v>2247</v>
       </c>
       <c r="AR38" s="14" t="s">
         <v>2077</v>
@@ -29511,7 +29511,7 @@
         <v>2075</v>
       </c>
       <c r="AV38" s="14" t="s">
-        <v>2305</v>
+        <v>2303</v>
       </c>
       <c r="AW38" s="3" t="s">
         <v>2063</v>
@@ -29523,19 +29523,19 @@
         <v>2073</v>
       </c>
       <c r="AZ38" s="25" t="s">
-        <v>2407</v>
+        <v>2405</v>
       </c>
       <c r="BA38" s="14" t="s">
         <v>2072</v>
       </c>
       <c r="BB38" s="14" t="s">
-        <v>2453</v>
+        <v>2451</v>
       </c>
       <c r="BC38" s="14" t="s">
         <v>2071</v>
       </c>
       <c r="BD38" s="14" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
       <c r="BE38" s="14" t="s">
         <v>2070</v>
@@ -29553,16 +29553,16 @@
         <v>1286</v>
       </c>
       <c r="BJ38" s="14" t="s">
-        <v>2454</v>
+        <v>2452</v>
       </c>
       <c r="BK38" s="14" t="s">
         <v>2067</v>
       </c>
       <c r="BL38" s="14" t="s">
-        <v>2470</v>
+        <v>2468</v>
       </c>
       <c r="BM38" s="14" t="s">
-        <v>2455</v>
+        <v>2453</v>
       </c>
       <c r="BN38" s="25" t="s">
         <v>2066</v>
@@ -29580,13 +29580,13 @@
         <v>2062</v>
       </c>
       <c r="BS38" s="14" t="s">
-        <v>2360</v>
+        <v>2358</v>
       </c>
       <c r="BT38" s="14" t="s">
         <v>2061</v>
       </c>
       <c r="BU38" s="14" t="s">
-        <v>2456</v>
+        <v>2454</v>
       </c>
       <c r="BV38" s="25" t="s">
         <v>2060</v>
@@ -29598,7 +29598,7 @@
         <v>2058</v>
       </c>
       <c r="BY38" s="14" t="s">
-        <v>2464</v>
+        <v>2462</v>
       </c>
       <c r="BZ38" s="14" t="s">
         <v>2057</v>
@@ -29625,7 +29625,7 @@
         <v>2051</v>
       </c>
       <c r="CH38" s="14" t="s">
-        <v>2250</v>
+        <v>2248</v>
       </c>
       <c r="CI38" s="25" t="s">
         <v>2050</v>
@@ -29637,13 +29637,13 @@
         <v>2048</v>
       </c>
       <c r="CL38" s="14" t="s">
-        <v>2436</v>
+        <v>2434</v>
       </c>
       <c r="CM38" s="14" t="s">
         <v>2047</v>
       </c>
       <c r="CN38" s="14" t="s">
-        <v>2465</v>
+        <v>2463</v>
       </c>
       <c r="CO38" s="14" t="s">
         <v>2046</v>
@@ -29658,7 +29658,7 @@
         <v>2043</v>
       </c>
       <c r="CS38" s="14" t="s">
-        <v>2375</v>
+        <v>2373</v>
       </c>
       <c r="CT38" s="14" t="s">
         <v>1286</v>
@@ -29670,13 +29670,13 @@
         <v>2041</v>
       </c>
       <c r="CW38" s="14" t="s">
+        <v>2455</v>
+      </c>
+      <c r="CX38" s="14" t="s">
+        <v>2372</v>
+      </c>
+      <c r="CY38" s="14" t="s">
         <v>2457</v>
-      </c>
-      <c r="CX38" s="14" t="s">
-        <v>2374</v>
-      </c>
-      <c r="CY38" s="14" t="s">
-        <v>2459</v>
       </c>
       <c r="CZ38" s="14" t="s">
         <v>2040</v>
@@ -29691,7 +29691,7 @@
         <v>2037</v>
       </c>
       <c r="DD38" s="14" t="s">
-        <v>2302</v>
+        <v>2300</v>
       </c>
       <c r="DE38" s="14" t="s">
         <v>2036</v>
@@ -29709,7 +29709,7 @@
         <v>1286</v>
       </c>
       <c r="DJ38" s="14" t="s">
-        <v>2251</v>
+        <v>2249</v>
       </c>
       <c r="DK38" s="3" t="s">
         <v>2034</v>
@@ -29721,7 +29721,7 @@
         <v>1286</v>
       </c>
       <c r="DN38" s="14" t="s">
-        <v>2466</v>
+        <v>2464</v>
       </c>
       <c r="DO38" s="25" t="s">
         <v>1286</v>
@@ -29730,7 +29730,7 @@
         <v>2032</v>
       </c>
       <c r="DQ38" s="14" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="DR38" s="14" t="s">
         <v>2031</v>
@@ -29775,7 +29775,7 @@
         <v>2020</v>
       </c>
       <c r="EF38" s="25" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
       <c r="EG38" s="14" t="s">
         <v>1286</v>
@@ -29790,7 +29790,7 @@
         <v>2019</v>
       </c>
       <c r="EK38" s="25" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="EL38" s="25" t="s">
         <v>1286</v>
@@ -29805,7 +29805,7 @@
         <v>2016</v>
       </c>
       <c r="EP38" s="14" t="s">
-        <v>2252</v>
+        <v>2250</v>
       </c>
       <c r="EQ38" s="14" t="s">
         <v>2015</v>
@@ -29817,7 +29817,7 @@
         <v>1286</v>
       </c>
       <c r="ET38" s="14" t="s">
-        <v>2460</v>
+        <v>2458</v>
       </c>
       <c r="EU38" s="25" t="s">
         <v>2014</v>
@@ -29835,22 +29835,22 @@
         <v>2010</v>
       </c>
       <c r="EZ38" s="14" t="s">
-        <v>2468</v>
+        <v>2466</v>
       </c>
       <c r="FA38" s="14" t="s">
+        <v>2459</v>
+      </c>
+      <c r="FB38" s="3" t="s">
         <v>2461</v>
       </c>
-      <c r="FB38" s="3" t="s">
-        <v>2463</v>
-      </c>
       <c r="FC38" s="14" t="s">
-        <v>2462</v>
+        <v>2460</v>
       </c>
       <c r="FD38" s="25" t="s">
         <v>2009</v>
       </c>
       <c r="FE38" s="14" t="s">
-        <v>2253</v>
+        <v>2251</v>
       </c>
       <c r="FF38" s="25" t="s">
         <v>2008</v>
@@ -29865,13 +29865,13 @@
         <v>2005</v>
       </c>
       <c r="FJ38" s="14" t="s">
-        <v>2254</v>
+        <v>2252</v>
       </c>
       <c r="FK38" s="14" t="s">
-        <v>2451</v>
+        <v>2449</v>
       </c>
       <c r="FL38" s="14" t="s">
-        <v>2431</v>
+        <v>2429</v>
       </c>
       <c r="FM38" s="14" t="s">
         <v>2004</v>
@@ -29961,12 +29961,12 @@
         <v>398</v>
       </c>
     </row>
-    <row r="39" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>2241</v>
+        <v>2239</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>1287</v>
@@ -29984,7 +29984,7 @@
         <v>1289</v>
       </c>
       <c r="H39" s="25" t="s">
-        <v>2367</v>
+        <v>2365</v>
       </c>
       <c r="I39" s="25" t="s">
         <v>1290</v>
@@ -29993,16 +29993,16 @@
         <v>1291</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>2415</v>
+        <v>2413</v>
       </c>
       <c r="L39" s="14" t="s">
+        <v>2484</v>
+      </c>
+      <c r="M39" s="25" t="s">
+        <v>2485</v>
+      </c>
+      <c r="N39" s="25" t="s">
         <v>2486</v>
-      </c>
-      <c r="M39" s="25" t="s">
-        <v>2487</v>
-      </c>
-      <c r="N39" s="25" t="s">
-        <v>2488</v>
       </c>
       <c r="O39" s="25" t="s">
         <v>1292</v>
@@ -30011,7 +30011,7 @@
         <v>398</v>
       </c>
       <c r="Q39" s="25" t="s">
-        <v>2489</v>
+        <v>2487</v>
       </c>
       <c r="R39" s="25" t="s">
         <v>1848</v>
@@ -30032,10 +30032,10 @@
         <v>1947</v>
       </c>
       <c r="X39" s="25" t="s">
-        <v>2490</v>
+        <v>2488</v>
       </c>
       <c r="Y39" s="25" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
       <c r="Z39" s="25" t="s">
         <v>1739</v>
@@ -30044,40 +30044,40 @@
         <v>1294</v>
       </c>
       <c r="AB39" s="25" t="s">
+        <v>2490</v>
+      </c>
+      <c r="AC39" s="25" t="s">
+        <v>2491</v>
+      </c>
+      <c r="AD39" s="25" t="s">
         <v>2492</v>
-      </c>
-      <c r="AC39" s="25" t="s">
-        <v>2493</v>
-      </c>
-      <c r="AD39" s="25" t="s">
-        <v>2494</v>
       </c>
       <c r="AE39" s="25" t="s">
         <v>1295</v>
       </c>
       <c r="AF39" s="25" t="s">
+        <v>2493</v>
+      </c>
+      <c r="AG39" s="25" t="s">
+        <v>2494</v>
+      </c>
+      <c r="AH39" s="44" t="s">
         <v>2495</v>
       </c>
-      <c r="AG39" s="25" t="s">
+      <c r="AI39" s="25" t="s">
         <v>2496</v>
-      </c>
-      <c r="AH39" s="44" t="s">
-        <v>2497</v>
-      </c>
-      <c r="AI39" s="25" t="s">
-        <v>2498</v>
       </c>
       <c r="AJ39" s="25" t="s">
         <v>1745</v>
       </c>
       <c r="AK39" s="25" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="AL39" s="25" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
       <c r="AM39" s="25" t="s">
-        <v>2324</v>
+        <v>2322</v>
       </c>
       <c r="AN39" s="25" t="s">
         <v>1772</v>
@@ -30086,58 +30086,58 @@
         <v>1626</v>
       </c>
       <c r="AP39" s="25" t="s">
+        <v>2499</v>
+      </c>
+      <c r="AQ39" s="25" t="s">
+        <v>2500</v>
+      </c>
+      <c r="AR39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AS39" s="25" t="s">
         <v>2501</v>
       </c>
-      <c r="AQ39" s="25" t="s">
+      <c r="AT39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AU39" s="25" t="s">
         <v>2502</v>
       </c>
-      <c r="AR39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="AS39" s="25" t="s">
+      <c r="AV39" s="25" t="s">
+        <v>2418</v>
+      </c>
+      <c r="AW39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AX39" s="25" t="s">
         <v>2503</v>
       </c>
-      <c r="AT39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="AU39" s="25" t="s">
+      <c r="AY39" s="25" t="s">
         <v>2504</v>
       </c>
-      <c r="AV39" s="25" t="s">
-        <v>2420</v>
-      </c>
-      <c r="AW39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="AX39" s="25" t="s">
-        <v>2505</v>
-      </c>
-      <c r="AY39" s="25" t="s">
-        <v>2506</v>
-      </c>
       <c r="AZ39" s="25" t="s">
-        <v>2392</v>
+        <v>2390</v>
       </c>
       <c r="BA39" s="25" t="s">
         <v>1506</v>
       </c>
       <c r="BB39" s="44" t="s">
+        <v>2505</v>
+      </c>
+      <c r="BC39" s="25" t="s">
+        <v>2506</v>
+      </c>
+      <c r="BD39" s="25" t="s">
         <v>2507</v>
       </c>
-      <c r="BC39" s="25" t="s">
+      <c r="BE39" s="25" t="s">
         <v>2508</v>
       </c>
-      <c r="BD39" s="25" t="s">
+      <c r="BF39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="BG39" s="25" t="s">
         <v>2509</v>
-      </c>
-      <c r="BE39" s="25" t="s">
-        <v>2510</v>
-      </c>
-      <c r="BF39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="BG39" s="25" t="s">
-        <v>2511</v>
       </c>
       <c r="BH39" s="25" t="s">
         <v>398</v>
@@ -30146,16 +30146,16 @@
         <v>1585</v>
       </c>
       <c r="BJ39" s="25" t="s">
+        <v>2510</v>
+      </c>
+      <c r="BK39" s="25" t="s">
+        <v>2511</v>
+      </c>
+      <c r="BL39" s="14" t="s">
         <v>2512</v>
       </c>
-      <c r="BK39" s="25" t="s">
+      <c r="BM39" s="25" t="s">
         <v>2513</v>
-      </c>
-      <c r="BL39" s="14" t="s">
-        <v>2514</v>
-      </c>
-      <c r="BM39" s="25" t="s">
-        <v>2515</v>
       </c>
       <c r="BN39" s="25" t="s">
         <v>1839</v>
@@ -30168,28 +30168,28 @@
         <v>398</v>
       </c>
       <c r="BR39" s="40" t="s">
+        <v>2514</v>
+      </c>
+      <c r="BS39" s="25" t="s">
+        <v>2515</v>
+      </c>
+      <c r="BT39" s="25" t="s">
         <v>2516</v>
       </c>
-      <c r="BS39" s="25" t="s">
+      <c r="BU39" s="25" t="s">
         <v>2517</v>
-      </c>
-      <c r="BT39" s="25" t="s">
-        <v>2518</v>
-      </c>
-      <c r="BU39" s="25" t="s">
-        <v>2519</v>
       </c>
       <c r="BV39" s="25" t="s">
         <v>1938</v>
       </c>
       <c r="BW39" s="25" t="s">
-        <v>2422</v>
+        <v>2420</v>
       </c>
       <c r="BX39" s="25" t="s">
-        <v>2520</v>
+        <v>2518</v>
       </c>
       <c r="BY39" s="25" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
       <c r="BZ39" s="25" t="s">
         <v>1512</v>
@@ -30198,7 +30198,7 @@
         <v>1599</v>
       </c>
       <c r="CB39" s="25" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="CC39" s="25" t="s">
         <v>398</v>
@@ -30213,85 +30213,85 @@
         <v>1477</v>
       </c>
       <c r="CG39" s="25" t="s">
+        <v>2521</v>
+      </c>
+      <c r="CH39" s="25" t="s">
+        <v>2522</v>
+      </c>
+      <c r="CI39" s="9" t="s">
         <v>2523</v>
-      </c>
-      <c r="CH39" s="25" t="s">
-        <v>2524</v>
-      </c>
-      <c r="CI39" s="9" t="s">
-        <v>2525</v>
       </c>
       <c r="CJ39" s="25" t="s">
         <v>1966</v>
       </c>
       <c r="CK39" s="25" t="s">
+        <v>2524</v>
+      </c>
+      <c r="CL39" s="25" t="s">
+        <v>2525</v>
+      </c>
+      <c r="CM39" s="25" t="s">
         <v>2526</v>
       </c>
-      <c r="CL39" s="25" t="s">
+      <c r="CN39" s="25" t="s">
         <v>2527</v>
-      </c>
-      <c r="CM39" s="25" t="s">
-        <v>2528</v>
-      </c>
-      <c r="CN39" s="25" t="s">
-        <v>2529</v>
       </c>
       <c r="CO39" s="25" t="s">
         <v>1655</v>
       </c>
       <c r="CP39" s="25" t="s">
-        <v>2424</v>
+        <v>2422</v>
       </c>
       <c r="CQ39" s="25" t="s">
+        <v>2528</v>
+      </c>
+      <c r="CR39" s="25" t="s">
+        <v>2529</v>
+      </c>
+      <c r="CS39" s="14" t="s">
         <v>2530</v>
       </c>
-      <c r="CR39" s="25" t="s">
+      <c r="CT39" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="CU39" s="25" t="s">
         <v>2531</v>
       </c>
-      <c r="CS39" s="14" t="s">
+      <c r="CV39" s="25" t="s">
         <v>2532</v>
       </c>
-      <c r="CT39" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="CU39" s="25" t="s">
+      <c r="CW39" s="25" t="s">
         <v>2533</v>
       </c>
-      <c r="CV39" s="25" t="s">
+      <c r="CX39" s="25" t="s">
         <v>2534</v>
       </c>
-      <c r="CW39" s="25" t="s">
+      <c r="CY39" s="25" t="s">
         <v>2535</v>
       </c>
-      <c r="CX39" s="25" t="s">
+      <c r="CZ39" s="25" t="s">
         <v>2536</v>
       </c>
-      <c r="CY39" s="25" t="s">
+      <c r="DA39" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="DB39" s="25" t="s">
         <v>2537</v>
       </c>
-      <c r="CZ39" s="25" t="s">
+      <c r="DC39" s="25" t="s">
         <v>2538</v>
       </c>
-      <c r="DA39" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="DB39" s="25" t="s">
+      <c r="DD39" s="25" t="s">
         <v>2539</v>
       </c>
-      <c r="DC39" s="25" t="s">
+      <c r="DE39" s="25" t="s">
         <v>2540</v>
       </c>
-      <c r="DD39" s="25" t="s">
+      <c r="DF39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="DG39" s="40" t="s">
         <v>2541</v>
-      </c>
-      <c r="DE39" s="25" t="s">
-        <v>2542</v>
-      </c>
-      <c r="DF39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="DG39" s="40" t="s">
-        <v>2543</v>
       </c>
       <c r="DH39" s="25" t="s">
         <v>398</v>
@@ -30306,52 +30306,52 @@
         <v>398</v>
       </c>
       <c r="DL39" s="25" t="s">
+        <v>2542</v>
+      </c>
+      <c r="DM39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="DN39" s="25" t="s">
+        <v>2543</v>
+      </c>
+      <c r="DO39" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="DP39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="DQ39" s="25" t="s">
         <v>2544</v>
       </c>
-      <c r="DM39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="DN39" s="25" t="s">
+      <c r="DR39" s="25" t="s">
         <v>2545</v>
-      </c>
-      <c r="DO39" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="DP39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="DQ39" s="25" t="s">
-        <v>2546</v>
-      </c>
-      <c r="DR39" s="25" t="s">
-        <v>2547</v>
       </c>
       <c r="DS39" s="25" t="s">
         <v>1912</v>
       </c>
       <c r="DT39" s="25" t="s">
+        <v>2546</v>
+      </c>
+      <c r="DU39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="DV39" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="DW39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="DX39" s="25" t="s">
+        <v>2547</v>
+      </c>
+      <c r="DY39" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="DZ39" s="25" t="s">
         <v>2548</v>
       </c>
-      <c r="DU39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="DV39" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="DW39" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="DX39" s="25" t="s">
+      <c r="EA39" s="25" t="s">
         <v>2549</v>
-      </c>
-      <c r="DY39" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="DZ39" s="25" t="s">
-        <v>2550</v>
-      </c>
-      <c r="EA39" s="25" t="s">
-        <v>2551</v>
       </c>
       <c r="EB39" s="25" t="s">
         <v>398</v>
@@ -30366,7 +30366,7 @@
         <v>1305</v>
       </c>
       <c r="EF39" s="25" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="EG39" s="25" t="s">
         <v>398</v>
@@ -30378,10 +30378,10 @@
         <v>398</v>
       </c>
       <c r="EJ39" s="25" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="EK39" s="25" t="s">
-        <v>2325</v>
+        <v>2323</v>
       </c>
       <c r="EL39" s="25" t="s">
         <v>398</v>
@@ -30390,13 +30390,13 @@
         <v>1935</v>
       </c>
       <c r="EN39" s="25" t="s">
+        <v>2552</v>
+      </c>
+      <c r="EO39" s="25" t="s">
+        <v>2553</v>
+      </c>
+      <c r="EP39" s="25" t="s">
         <v>2554</v>
-      </c>
-      <c r="EO39" s="25" t="s">
-        <v>2555</v>
-      </c>
-      <c r="EP39" s="25" t="s">
-        <v>2556</v>
       </c>
       <c r="EQ39" s="25" t="s">
         <v>1327</v>
@@ -30408,7 +30408,7 @@
         <v>398</v>
       </c>
       <c r="ET39" s="25" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
       <c r="EU39" s="25" t="s">
         <v>1663</v>
@@ -30420,40 +30420,40 @@
         <v>1923</v>
       </c>
       <c r="EX39" s="25" t="s">
-        <v>2427</v>
+        <v>2425</v>
       </c>
       <c r="EY39" s="25" t="s">
+        <v>2556</v>
+      </c>
+      <c r="EZ39" s="25" t="s">
+        <v>2557</v>
+      </c>
+      <c r="FA39" s="25" t="s">
         <v>2558</v>
       </c>
-      <c r="EZ39" s="25" t="s">
+      <c r="FB39" s="3" t="s">
         <v>2559</v>
       </c>
-      <c r="FA39" s="25" t="s">
+      <c r="FC39" s="40" t="s">
         <v>2560</v>
       </c>
-      <c r="FB39" s="3" t="s">
+      <c r="FD39" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="FE39" s="25" t="s">
         <v>2561</v>
-      </c>
-      <c r="FC39" s="40" t="s">
-        <v>2562</v>
-      </c>
-      <c r="FD39" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="FE39" s="25" t="s">
-        <v>2563</v>
       </c>
       <c r="FF39" s="25" t="s">
         <v>1843</v>
       </c>
       <c r="FG39" s="25" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="FH39" s="25" t="s">
         <v>1525</v>
       </c>
       <c r="FI39" s="25" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="FJ39" s="25" t="s">
         <v>1671</v>
@@ -30462,7 +30462,7 @@
         <v>1296</v>
       </c>
       <c r="FL39" s="25" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="FM39" s="45" t="s">
         <v>1565</v>
@@ -30552,9 +30552,9 @@
         <v>398</v>
       </c>
     </row>
-    <row r="40" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="55" t="s">
-        <v>2450</v>
+        <v>2448</v>
       </c>
       <c r="B40" s="55"/>
       <c r="C40" s="55"/>
@@ -30762,7 +30762,7 @@
       <c r="GN40" s="55"/>
       <c r="GO40" s="55"/>
     </row>
-    <row r="41" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>744</v>
       </c>
@@ -30770,7 +30770,7 @@
         <v>715</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>2340</v>
+        <v>2338</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>1269</v>
@@ -30779,19 +30779,19 @@
         <v>1273</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>2416</v>
+        <v>2414</v>
       </c>
       <c r="M41" s="27" t="s">
         <v>1951</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>2385</v>
+        <v>2383</v>
       </c>
       <c r="O41" s="5" t="s">
         <v>1281</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>2357</v>
+        <v>2355</v>
       </c>
       <c r="R41" s="5" t="s">
         <v>1849</v>
@@ -30815,7 +30815,7 @@
         <v>1532</v>
       </c>
       <c r="AC41" s="34" t="s">
-        <v>2358</v>
+        <v>2356</v>
       </c>
       <c r="AD41" s="5" t="s">
         <v>1232</v>
@@ -30848,7 +30848,7 @@
         <v>1898</v>
       </c>
       <c r="AZ41" s="5" t="s">
-        <v>2391</v>
+        <v>2389</v>
       </c>
       <c r="BA41" s="5" t="s">
         <v>1508</v>
@@ -30890,7 +30890,7 @@
         <v>1337</v>
       </c>
       <c r="BW41" s="5" t="s">
-        <v>2421</v>
+        <v>2419</v>
       </c>
       <c r="BX41" s="5" t="s">
         <v>857</v>
@@ -30900,7 +30900,7 @@
         <v>1766</v>
       </c>
       <c r="CI41" s="5" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="CJ41" s="5" t="s">
         <v>2187</v>
@@ -30909,28 +30909,28 @@
         <v>1835</v>
       </c>
       <c r="CL41" s="5" t="s">
-        <v>2434</v>
+        <v>2432</v>
       </c>
       <c r="CM41" s="5" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="CN41" s="5" t="s">
         <v>1818</v>
       </c>
       <c r="CP41" s="5" t="s">
-        <v>2423</v>
+        <v>2421</v>
       </c>
       <c r="CQ41" s="5" t="s">
         <v>1867</v>
       </c>
       <c r="CS41" s="5" t="s">
-        <v>2369</v>
+        <v>2367</v>
       </c>
       <c r="CW41" s="5" t="s">
         <v>1341</v>
       </c>
       <c r="CX41" s="16" t="s">
-        <v>2372</v>
+        <v>2370</v>
       </c>
       <c r="DB41" s="5" t="s">
         <v>1548</v>
@@ -30969,13 +30969,13 @@
         <v>1030</v>
       </c>
       <c r="EF41" s="5" t="s">
-        <v>2364</v>
+        <v>2362</v>
       </c>
       <c r="EJ41" s="5" t="s">
         <v>1373</v>
       </c>
       <c r="EK41" s="5" t="s">
-        <v>2306</v>
+        <v>2304</v>
       </c>
       <c r="EM41" s="5" t="s">
         <v>1934</v>
@@ -30987,7 +30987,7 @@
         <v>1328</v>
       </c>
       <c r="ES41" s="5" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="ET41" s="5" t="s">
         <v>1197</v>
@@ -31014,7 +31014,7 @@
         <v>1616</v>
       </c>
       <c r="FG41" s="5" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
       <c r="FH41" s="5" t="s">
         <v>1526</v>
@@ -31023,12 +31023,12 @@
         <v>1414</v>
       </c>
       <c r="FK41" s="5" t="s">
-        <v>2452</v>
+        <v>2450</v>
       </c>
     </row>
-    <row r="42" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>2242</v>
+        <v>2240</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>2205</v>
@@ -31052,7 +31052,7 @@
         <v>2208</v>
       </c>
       <c r="AC42" s="34" t="s">
-        <v>2447</v>
+        <v>2445</v>
       </c>
       <c r="AH42" s="5" t="s">
         <v>1991</v>
@@ -31070,22 +31070,22 @@
         <v>1965</v>
       </c>
       <c r="CL42" s="16" t="s">
-        <v>2433</v>
+        <v>2431</v>
       </c>
       <c r="CS42" s="5" t="s">
-        <v>2292</v>
+        <v>2290</v>
       </c>
       <c r="CX42" s="5" t="s">
-        <v>2373</v>
+        <v>2371</v>
       </c>
       <c r="CY42" s="5" t="s">
         <v>1961</v>
       </c>
       <c r="DK42" s="53" t="s">
-        <v>2432</v>
+        <v>2430</v>
       </c>
       <c r="DN42" s="54" t="s">
-        <v>2435</v>
+        <v>2433</v>
       </c>
       <c r="DS42" s="14" t="s">
         <v>1911</v>
@@ -31103,7 +31103,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="43" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:197" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
         <v>709</v>
       </c>

</xml_diff>